<commit_message>
tests, fix nav bar, trouver lang translate
</commit_message>
<xml_diff>
--- a/semaine 9/Feuille_de_temps_S1-Eq1.xlsx
+++ b/semaine 9/Feuille_de_temps_S1-Eq1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_web\CoolKidsClub-Gym\semaine 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623AE24B-58D4-4630-BD81-4A04E440E384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879F3995-598C-406B-9A80-6AB76AACDABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="326" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="99">
   <si>
     <t>Temps</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>UI general du site</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Apprendre Jest</t>
+  </si>
+  <si>
+    <t>trouver language</t>
+  </si>
+  <si>
+    <t>Fix barre de navigation (choses affichent correctement, logo ne se traduit pas)</t>
+  </si>
+  <si>
+    <t>Creation test unitaire</t>
+  </si>
+  <si>
+    <t>Tester connection</t>
+  </si>
+  <si>
+    <t>Tester creation compte</t>
+  </si>
+  <si>
+    <t>Tester ajouter article</t>
   </si>
 </sst>
 </file>
@@ -1391,15 +1415,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P1000"/>
+  <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1448,8 +1472,14 @@
       <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>12</v>
       </c>
@@ -1483,8 +1513,14 @@
       <c r="P2" s="13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="Q2" s="13">
+        <v>3</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1518,8 +1554,14 @@
       <c r="P3" s="13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>3.5</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="2">
         <v>0.5</v>
@@ -1548,8 +1590,14 @@
       <c r="P4" s="13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>2.5</v>
+      </c>
+      <c r="R4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="2">
         <v>0.5</v>
@@ -1578,8 +1626,14 @@
       <c r="P5" s="13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>1.5</v>
+      </c>
+      <c r="R5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="2">
         <v>1</v>
@@ -1596,183 +1650,155 @@
       <c r="P6" s="13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="F7" s="12"/>
       <c r="H7" s="12"/>
       <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="12"/>
       <c r="H8" s="12"/>
       <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="D9" s="12"/>
       <c r="F9" s="12"/>
       <c r="H9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
       <c r="F11" s="12"/>
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
       <c r="F12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12"/>
       <c r="D13" s="12"/>
       <c r="F13" s="12"/>
       <c r="H13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="F14" s="12"/>
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
       <c r="D15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="J15" s="12"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="12"/>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="12"/>
       <c r="D28" s="12"/>
       <c r="F28" s="12"/>
       <c r="H28" s="12"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
       <c r="D29" s="12"/>
       <c r="F29" s="12"/>
       <c r="H29" s="12"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="12"/>
       <c r="D30" s="12"/>
       <c r="F30" s="12"/>
       <c r="H30" s="12"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="12"/>
       <c r="D31" s="12"/>
       <c r="F31" s="12"/>
       <c r="H31" s="12"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="12"/>
       <c r="D32" s="12"/>
       <c r="F32" s="12"/>

</xml_diff>